<commit_message>
Stock Ratings - update input xlsx file / updtae main
</commit_message>
<xml_diff>
--- a/Column_A_positions.xlsx
+++ b/Column_A_positions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biacarvalheira/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biacarvalheira/Desktop/Stock_Ratings_Scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBCB1E1-EC07-5940-8D31-A7E9C9EC234C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DB866D-2FED-BD42-B57F-366B46689A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{BF2ED942-5559-7448-97FA-D6A9EB14A6F4}"/>
   </bookViews>
@@ -44,12 +44,6 @@
     <t>abnb</t>
   </si>
   <si>
-    <t>ael-a</t>
-  </si>
-  <si>
-    <t>all-i</t>
-  </si>
-  <si>
     <t>amd</t>
   </si>
   <si>
@@ -155,9 +149,6 @@
     <t>efc</t>
   </si>
   <si>
-    <t>efc-b</t>
-  </si>
-  <si>
     <t>el</t>
   </si>
   <si>
@@ -185,9 +176,6 @@
     <t>frc</t>
   </si>
   <si>
-    <t>frc-n</t>
-  </si>
-  <si>
     <t>fxi</t>
   </si>
   <si>
@@ -332,9 +320,6 @@
     <t>snv</t>
   </si>
   <si>
-    <t>snv-e</t>
-  </si>
-  <si>
     <t>spce</t>
   </si>
   <si>
@@ -399,6 +384,21 @@
   </si>
   <si>
     <t>sbny</t>
+  </si>
+  <si>
+    <t>AEL'A</t>
+  </si>
+  <si>
+    <t>all'i</t>
+  </si>
+  <si>
+    <t>efc'b</t>
+  </si>
+  <si>
+    <t>frc'n</t>
+  </si>
+  <si>
+    <t>snv'e</t>
   </si>
 </sst>
 </file>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA2B5F9-20ED-4F45-B304-799F76A8AB6C}">
   <dimension ref="A1:A2265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,592 +834,592 @@
     </row>
     <row r="3" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>2</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="9" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="9" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" s="9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" s="9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="9" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A111" s="9" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A112" s="9" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A113" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="8" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
@@ -1541,7 +1541,7 @@
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Stock Ratings - add - current working version - no warning messages
</commit_message>
<xml_diff>
--- a/Column_A_positions.xlsx
+++ b/Column_A_positions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/biacarvalheira/Desktop/Stock_Ratings_Scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DB866D-2FED-BD42-B57F-366B46689A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27460A34-13A9-B742-BAE8-4488B75BA6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{BF2ED942-5559-7448-97FA-D6A9EB14A6F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>aapl</t>
   </si>
@@ -59,330 +59,6 @@
     <t>arkx</t>
   </si>
   <si>
-    <t>asml</t>
-  </si>
-  <si>
-    <t>asts</t>
-  </si>
-  <si>
-    <t>baba</t>
-  </si>
-  <si>
-    <t>bac</t>
-  </si>
-  <si>
-    <t>betz</t>
-  </si>
-  <si>
-    <t>bmbl</t>
-  </si>
-  <si>
-    <t>bmez</t>
-  </si>
-  <si>
-    <t>brk.b</t>
-  </si>
-  <si>
-    <t>bstz</t>
-  </si>
-  <si>
-    <t>btcusd</t>
-  </si>
-  <si>
-    <t>bud</t>
-  </si>
-  <si>
-    <t>bx</t>
-  </si>
-  <si>
-    <t>bxp</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>carr</t>
-  </si>
-  <si>
-    <t>cat</t>
-  </si>
-  <si>
-    <t>coin</t>
-  </si>
-  <si>
-    <t>cour</t>
-  </si>
-  <si>
-    <t>crwd</t>
-  </si>
-  <si>
-    <t>csco</t>
-  </si>
-  <si>
-    <t>ctra</t>
-  </si>
-  <si>
-    <t>cybr</t>
-  </si>
-  <si>
-    <t>dal</t>
-  </si>
-  <si>
-    <t>dhi</t>
-  </si>
-  <si>
-    <t>dis</t>
-  </si>
-  <si>
-    <t>dvn</t>
-  </si>
-  <si>
-    <t>edoc</t>
-  </si>
-  <si>
-    <t>edr</t>
-  </si>
-  <si>
-    <t>edut</t>
-  </si>
-  <si>
-    <t>efc</t>
-  </si>
-  <si>
-    <t>el</t>
-  </si>
-  <si>
-    <t>ethusd</t>
-  </si>
-  <si>
-    <t>expe</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>fcnco</t>
-  </si>
-  <si>
-    <t>fitb</t>
-  </si>
-  <si>
-    <t>fl</t>
-  </si>
-  <si>
-    <t>frbc</t>
-  </si>
-  <si>
-    <t>frc</t>
-  </si>
-  <si>
-    <t>fxi</t>
-  </si>
-  <si>
-    <t>gbtc</t>
-  </si>
-  <si>
-    <t>gnrc</t>
-  </si>
-  <si>
-    <t>googl</t>
-  </si>
-  <si>
-    <t>gs</t>
-  </si>
-  <si>
-    <t>gxc</t>
-  </si>
-  <si>
-    <t>hal</t>
-  </si>
-  <si>
-    <t>ibb</t>
-  </si>
-  <si>
-    <t>ifn</t>
-  </si>
-  <si>
-    <t>jpm</t>
-  </si>
-  <si>
-    <t>kbe</t>
-  </si>
-  <si>
-    <t>kmi</t>
-  </si>
-  <si>
-    <t>kweb</t>
-  </si>
-  <si>
-    <t>li</t>
-  </si>
-  <si>
-    <t>luv</t>
-  </si>
-  <si>
-    <t>meta</t>
-  </si>
-  <si>
-    <t>mmd</t>
-  </si>
-  <si>
-    <t>mrna</t>
-  </si>
-  <si>
-    <t>mrvl</t>
-  </si>
-  <si>
-    <t>ms</t>
-  </si>
-  <si>
-    <t>msft</t>
-  </si>
-  <si>
-    <t>mtch</t>
-  </si>
-  <si>
-    <t>nflx</t>
-  </si>
-  <si>
-    <t>nio</t>
-  </si>
-  <si>
-    <t>nly</t>
-  </si>
-  <si>
-    <t>nvda</t>
-  </si>
-  <si>
-    <t>para</t>
-  </si>
-  <si>
-    <t>pbs</t>
-  </si>
-  <si>
-    <t>penn</t>
-  </si>
-  <si>
-    <t>pfe</t>
-  </si>
-  <si>
-    <t>potx</t>
-  </si>
-  <si>
-    <t>psq</t>
-  </si>
-  <si>
-    <t>pton</t>
-  </si>
-  <si>
-    <t>pxd</t>
-  </si>
-  <si>
-    <t>pypl</t>
-  </si>
-  <si>
-    <t>qcom</t>
-  </si>
-  <si>
-    <t>qqq</t>
-  </si>
-  <si>
-    <t>qqqj</t>
-  </si>
-  <si>
-    <t>qqqs</t>
-  </si>
-  <si>
-    <t>ritm</t>
-  </si>
-  <si>
-    <t>rklb</t>
-  </si>
-  <si>
-    <t>rprx</t>
-  </si>
-  <si>
-    <t>save</t>
-  </si>
-  <si>
-    <t>schw</t>
-  </si>
-  <si>
-    <t>sh</t>
-  </si>
-  <si>
-    <t>snap</t>
-  </si>
-  <si>
-    <t>snow</t>
-  </si>
-  <si>
-    <t>snv</t>
-  </si>
-  <si>
-    <t>spce</t>
-  </si>
-  <si>
-    <t>spir</t>
-  </si>
-  <si>
-    <t>ssss</t>
-  </si>
-  <si>
-    <t>tdoc</t>
-  </si>
-  <si>
-    <t>tost</t>
-  </si>
-  <si>
-    <t>tqqq</t>
-  </si>
-  <si>
-    <t>tsla</t>
-  </si>
-  <si>
-    <t>ua</t>
-  </si>
-  <si>
-    <t>ual</t>
-  </si>
-  <si>
-    <t>uber</t>
-  </si>
-  <si>
-    <t>ubs</t>
-  </si>
-  <si>
-    <t>udmy</t>
-  </si>
-  <si>
-    <t>vaxx</t>
-  </si>
-  <si>
-    <t>vorbq</t>
-  </si>
-  <si>
-    <t>vz</t>
-  </si>
-  <si>
-    <t>wbd</t>
-  </si>
-  <si>
-    <t>wfc</t>
-  </si>
-  <si>
-    <t>xbi</t>
-  </si>
-  <si>
-    <t>xle</t>
-  </si>
-  <si>
-    <t>xpev</t>
-  </si>
-  <si>
-    <t>zm</t>
-  </si>
-  <si>
     <t>sbny</t>
   </si>
   <si>
@@ -390,15 +66,6 @@
   </si>
   <si>
     <t>all'i</t>
-  </si>
-  <si>
-    <t>efc'b</t>
-  </si>
-  <si>
-    <t>frc'n</t>
-  </si>
-  <si>
-    <t>snv'e</t>
   </si>
 </sst>
 </file>
@@ -813,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA2B5F9-20ED-4F45-B304-799F76A8AB6C}">
   <dimension ref="A1:A2265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A10:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -834,12 +501,12 @@
     </row>
     <row r="3" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>117</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
@@ -868,559 +535,337 @@
       </c>
     </row>
     <row r="10" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>7</v>
-      </c>
+      <c r="A10" s="6"/>
     </row>
     <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="A11" s="9"/>
     </row>
     <row r="12" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="A13" s="7"/>
     </row>
     <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="A14" s="9"/>
     </row>
     <row r="15" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>12</v>
-      </c>
+      <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="A17" s="7"/>
     </row>
     <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
-        <v>15</v>
-      </c>
+      <c r="A18" s="9"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="A19" s="8"/>
     </row>
     <row r="20" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="A20" s="6"/>
     </row>
     <row r="21" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A22" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="A22" s="9"/>
     </row>
     <row r="23" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>20</v>
-      </c>
+      <c r="A23" s="6"/>
     </row>
     <row r="24" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="A24" s="6"/>
     </row>
     <row r="25" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>22</v>
-      </c>
+      <c r="A25" s="6"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>23</v>
-      </c>
+      <c r="A26" s="7"/>
     </row>
     <row r="27" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="A27" s="6"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="A28" s="8"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="A29" s="8"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="A30" s="8"/>
     </row>
     <row r="31" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="A31" s="6"/>
     </row>
     <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A32" s="9" t="s">
-        <v>29</v>
-      </c>
+      <c r="A32" s="9"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="A33" s="7"/>
     </row>
     <row r="34" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="A34" s="6"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>32</v>
-      </c>
+      <c r="A35" s="7"/>
     </row>
     <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A36" s="9" t="s">
-        <v>33</v>
-      </c>
+      <c r="A36" s="9"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="A37" s="7"/>
     </row>
     <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="A38" s="9"/>
     </row>
     <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="A39" s="9"/>
     </row>
     <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A40" s="9" t="s">
-        <v>118</v>
-      </c>
+      <c r="A40" s="9"/>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="A41" s="8"/>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="A42" s="8"/>
     </row>
     <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A43" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="A43" s="9"/>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="A44" s="7"/>
     </row>
     <row r="45" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="A45" s="6"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="A46" s="7"/>
     </row>
     <row r="47" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="A47" s="6"/>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
-        <v>44</v>
-      </c>
+      <c r="A48" s="7"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="A49" s="7"/>
     </row>
     <row r="50" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>119</v>
-      </c>
+      <c r="A50" s="6"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
-        <v>46</v>
-      </c>
+      <c r="A51" s="7"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="7" t="s">
-        <v>47</v>
-      </c>
+      <c r="A52" s="7"/>
     </row>
     <row r="53" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
-        <v>48</v>
-      </c>
+      <c r="A53" s="6"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
-        <v>49</v>
-      </c>
+      <c r="A54" s="7"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="A55" s="7"/>
     </row>
     <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A56" s="9" t="s">
-        <v>51</v>
-      </c>
+      <c r="A56" s="9"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
-        <v>52</v>
-      </c>
+      <c r="A57" s="8"/>
     </row>
     <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A58" s="9" t="s">
-        <v>53</v>
-      </c>
+      <c r="A58" s="9"/>
     </row>
     <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A59" s="9" t="s">
-        <v>54</v>
-      </c>
+      <c r="A59" s="9"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="8" t="s">
-        <v>55</v>
-      </c>
+      <c r="A60" s="8"/>
     </row>
     <row r="61" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
-        <v>56</v>
-      </c>
+      <c r="A61" s="6"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="7" t="s">
-        <v>57</v>
-      </c>
+      <c r="A62" s="7"/>
     </row>
     <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A63" s="9" t="s">
-        <v>58</v>
-      </c>
+      <c r="A63" s="9"/>
     </row>
     <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A64" s="9" t="s">
-        <v>59</v>
-      </c>
+      <c r="A64" s="9"/>
     </row>
     <row r="65" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>60</v>
-      </c>
+      <c r="A65" s="6"/>
     </row>
     <row r="66" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="A66" s="6"/>
     </row>
     <row r="67" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
-        <v>62</v>
-      </c>
+      <c r="A67" s="6"/>
     </row>
     <row r="68" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
-        <v>63</v>
-      </c>
+      <c r="A68" s="6"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="A69" s="7"/>
     </row>
     <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A70" s="9" t="s">
-        <v>65</v>
-      </c>
+      <c r="A70" s="9"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="7" t="s">
-        <v>66</v>
-      </c>
+      <c r="A71" s="7"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="7" t="s">
-        <v>67</v>
-      </c>
+      <c r="A72" s="7"/>
     </row>
     <row r="73" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
-        <v>68</v>
-      </c>
+      <c r="A73" s="6"/>
     </row>
     <row r="74" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
-        <v>69</v>
-      </c>
+      <c r="A74" s="6"/>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="7" t="s">
-        <v>70</v>
-      </c>
+      <c r="A75" s="7"/>
     </row>
     <row r="76" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>71</v>
-      </c>
+      <c r="A76" s="6"/>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="8" t="s">
-        <v>72</v>
-      </c>
+      <c r="A77" s="8"/>
     </row>
     <row r="78" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A78" s="6" t="s">
-        <v>73</v>
-      </c>
+      <c r="A78" s="6"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="A79" s="7"/>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="7" t="s">
-        <v>75</v>
-      </c>
+      <c r="A80" s="7"/>
     </row>
     <row r="81" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A81" s="9" t="s">
-        <v>76</v>
-      </c>
+      <c r="A81" s="9"/>
     </row>
     <row r="82" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A82" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="A82" s="6"/>
     </row>
     <row r="83" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A83" s="9" t="s">
-        <v>78</v>
-      </c>
+      <c r="A83" s="9"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="7" t="s">
-        <v>79</v>
-      </c>
+      <c r="A84" s="7"/>
     </row>
     <row r="85" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A85" s="6" t="s">
-        <v>80</v>
-      </c>
+      <c r="A85" s="6"/>
     </row>
     <row r="86" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
-        <v>81</v>
-      </c>
+      <c r="A86" s="6"/>
     </row>
     <row r="87" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A87" s="6" t="s">
-        <v>82</v>
-      </c>
+      <c r="A87" s="6"/>
     </row>
     <row r="88" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A88" s="9" t="s">
-        <v>83</v>
-      </c>
+      <c r="A88" s="9"/>
     </row>
     <row r="89" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A89" s="9" t="s">
-        <v>84</v>
-      </c>
+      <c r="A89" s="9"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90" s="7" t="s">
-        <v>85</v>
-      </c>
+      <c r="A90" s="7"/>
     </row>
     <row r="91" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A91" s="9" t="s">
-        <v>86</v>
-      </c>
+      <c r="A91" s="9"/>
     </row>
     <row r="92" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A92" s="6" t="s">
-        <v>87</v>
-      </c>
+      <c r="A92" s="6"/>
     </row>
     <row r="93" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A93" s="6" t="s">
-        <v>88</v>
-      </c>
+      <c r="A93" s="6"/>
     </row>
     <row r="94" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
-        <v>89</v>
-      </c>
+      <c r="A94" s="6"/>
     </row>
     <row r="95" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="A95" s="6"/>
     </row>
     <row r="96" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A96" s="6" t="s">
-        <v>91</v>
-      </c>
+      <c r="A96" s="6"/>
     </row>
     <row r="97" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
-        <v>92</v>
-      </c>
+      <c r="A97" s="6"/>
     </row>
     <row r="98" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A98" s="6" t="s">
-        <v>93</v>
-      </c>
+      <c r="A98" s="6"/>
     </row>
     <row r="99" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A99" s="6" t="s">
-        <v>120</v>
-      </c>
+      <c r="A99" s="6"/>
     </row>
     <row r="100" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A100" s="9" t="s">
-        <v>94</v>
-      </c>
+      <c r="A100" s="9"/>
     </row>
     <row r="101" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A101" s="9" t="s">
-        <v>95</v>
-      </c>
+      <c r="A101" s="9"/>
     </row>
     <row r="102" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A102" s="6" t="s">
-        <v>96</v>
-      </c>
+      <c r="A102" s="6"/>
     </row>
     <row r="103" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A103" s="9" t="s">
-        <v>97</v>
-      </c>
+      <c r="A103" s="9"/>
     </row>
     <row r="104" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A104" s="6" t="s">
-        <v>98</v>
-      </c>
+      <c r="A104" s="6"/>
     </row>
     <row r="105" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A105" s="6" t="s">
-        <v>99</v>
-      </c>
+      <c r="A105" s="6"/>
     </row>
     <row r="106" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A106" s="9" t="s">
-        <v>100</v>
-      </c>
+      <c r="A106" s="9"/>
     </row>
     <row r="107" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A107" s="9" t="s">
-        <v>101</v>
-      </c>
+      <c r="A107" s="9"/>
     </row>
     <row r="108" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A108" s="9" t="s">
-        <v>102</v>
-      </c>
+      <c r="A108" s="9"/>
     </row>
     <row r="109" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A109" s="9" t="s">
-        <v>103</v>
-      </c>
+      <c r="A109" s="9"/>
     </row>
     <row r="110" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A110" s="6" t="s">
-        <v>104</v>
-      </c>
+      <c r="A110" s="6"/>
     </row>
     <row r="111" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A111" s="9" t="s">
-        <v>105</v>
-      </c>
+      <c r="A111" s="9"/>
     </row>
     <row r="112" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A112" s="9" t="s">
-        <v>106</v>
-      </c>
+      <c r="A112" s="9"/>
     </row>
     <row r="113" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A113" s="9" t="s">
-        <v>107</v>
-      </c>
+      <c r="A113" s="9"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" s="8" t="s">
-        <v>108</v>
-      </c>
+      <c r="A114" s="8"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" s="8" t="s">
-        <v>109</v>
-      </c>
+      <c r="A115" s="8"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116" s="7" t="s">
-        <v>110</v>
-      </c>
+      <c r="A116" s="7"/>
     </row>
     <row r="117" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A117" s="6" t="s">
-        <v>111</v>
-      </c>
+      <c r="A117" s="6"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118" s="7" t="s">
-        <v>112</v>
-      </c>
+      <c r="A118" s="7"/>
     </row>
     <row r="119" spans="1:1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A119" s="6" t="s">
-        <v>113</v>
-      </c>
+      <c r="A119" s="6"/>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120" s="7" t="s">
-        <v>114</v>
-      </c>
+      <c r="A120" s="7"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
@@ -1541,7 +986,7 @@
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" s="7" t="s">
-        <v>115</v>
+        <v>7</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>